<commit_message>
updated alternate dish names based on comments from nutritionist
</commit_message>
<xml_diff>
--- a/dishes_db.xlsx
+++ b/dishes_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rochiecuevas/Documents/IRRI/DATA/DFC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ABBBD1-8C09-0C4D-BC0B-C9868ABD78C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADF8844-01A2-484F-86EB-FE2F1F4F20C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="460" windowWidth="25440" windowHeight="14580" activeTab="2" xr2:uid="{C5627AB3-2530-1846-A42E-E8DBFFAB0086}"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="14580" activeTab="4" xr2:uid="{C5627AB3-2530-1846-A42E-E8DBFFAB0086}"/>
   </bookViews>
   <sheets>
     <sheet name="states" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4263" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4266" uniqueCount="613">
   <si>
     <t>Id</t>
   </si>
@@ -1866,6 +1866,12 @@
   </si>
   <si>
     <t>puffed rice immersed in water</t>
+  </si>
+  <si>
+    <t>Sooji upma</t>
+  </si>
+  <si>
+    <t>thick porridge made of dry roasted semolina</t>
   </si>
 </sst>
 </file>
@@ -2406,10 +2412,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060BD633-8C73-7A4F-B89C-EC94C4D86C07}">
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4140,6 +4146,20 @@
         <v>266</v>
       </c>
     </row>
+    <row r="124" spans="1:4">
+      <c r="A124">
+        <v>135</v>
+      </c>
+      <c r="B124" t="s">
+        <v>611</v>
+      </c>
+      <c r="C124" t="s">
+        <v>612</v>
+      </c>
+      <c r="D124" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D123" xr:uid="{E2EF74E5-8514-F148-8476-989D83D2F4DF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4150,8 +4170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D9E83B-6AF3-F442-A900-2FF427687D74}">
   <dimension ref="A1:F214"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F215"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4532,7 +4552,7 @@
         <v>294</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -5229,7 +5249,7 @@
         <v>324</v>
       </c>
       <c r="E63" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -7811,8 +7831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9379C13F-7094-084A-ACF5-EBA14959B870}">
   <dimension ref="A1:F1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1003" sqref="E1003"/>
+    <sheetView tabSelected="1" topLeftCell="A865" workbookViewId="0">
+      <selection activeCell="B875" sqref="B875"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -25407,7 +25427,7 @@
         <v>921</v>
       </c>
       <c r="B880" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C880" t="s">
         <v>540</v>
@@ -25427,7 +25447,7 @@
         <v>922</v>
       </c>
       <c r="B881" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C881" t="s">
         <v>456</v>
@@ -25447,7 +25467,7 @@
         <v>923</v>
       </c>
       <c r="B882" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C882" t="s">
         <v>479</v>
@@ -25467,7 +25487,7 @@
         <v>924</v>
       </c>
       <c r="B883" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C883" t="s">
         <v>427</v>
@@ -25487,7 +25507,7 @@
         <v>925</v>
       </c>
       <c r="B884" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C884" t="s">
         <v>429</v>
@@ -25507,7 +25527,7 @@
         <v>926</v>
       </c>
       <c r="B885" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C885" t="s">
         <v>492</v>
@@ -25527,7 +25547,7 @@
         <v>927</v>
       </c>
       <c r="B886" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C886" t="s">
         <v>493</v>
@@ -25547,7 +25567,7 @@
         <v>928</v>
       </c>
       <c r="B887" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C887" t="s">
         <v>417</v>
@@ -25567,7 +25587,7 @@
         <v>929</v>
       </c>
       <c r="B888" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C888" t="s">
         <v>410</v>
@@ -25587,7 +25607,7 @@
         <v>930</v>
       </c>
       <c r="B889" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C889" t="s">
         <v>480</v>
@@ -25607,7 +25627,7 @@
         <v>931</v>
       </c>
       <c r="B890" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C890" t="s">
         <v>424</v>
@@ -25627,7 +25647,7 @@
         <v>932</v>
       </c>
       <c r="B891" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C891" t="s">
         <v>412</v>
@@ -25647,7 +25667,7 @@
         <v>933</v>
       </c>
       <c r="B892" t="s">
-        <v>70</v>
+        <v>611</v>
       </c>
       <c r="C892" t="s">
         <v>454</v>

</xml_diff>